<commit_message>
Wijziging: Grafieken verplaatst naar Beschrijvend. Toegevoegd: opgaven beschrijvend/
</commit_message>
<xml_diff>
--- a/_book/data/tablets.xlsx
+++ b/_book/data/tablets.xlsx
@@ -1,19 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\studieboeken\excelanalyse\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F8A467F-8643-47A7-A121-E464BA55B53E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14C5A25-F2CB-49C6-873C-1DA36A2FD56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C90250F-73E2-4CA5-8653-F75E95E8909B}"/>
   </bookViews>
   <sheets>
-    <sheet name="tablets" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -397,10 +392,13 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="7.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -415,115 +413,116 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1020</v>
+        <v>51</v>
       </c>
       <c r="B2">
-        <v>840</v>
+        <v>42</v>
       </c>
       <c r="C2">
-        <v>1430</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1560</v>
+        <v>78</v>
       </c>
       <c r="B3">
-        <v>940</v>
+        <v>47</v>
       </c>
       <c r="C3">
-        <v>1750</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>560</v>
+        <v>28</v>
       </c>
       <c r="B4">
-        <v>780</v>
+        <v>39</v>
       </c>
       <c r="C4">
-        <v>870</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>780</v>
+        <v>39</v>
       </c>
       <c r="B5">
-        <v>650</v>
+        <v>33</v>
       </c>
       <c r="C5">
-        <v>920</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>990</v>
+        <v>50</v>
       </c>
       <c r="B6">
-        <v>720</v>
+        <v>36</v>
       </c>
       <c r="C6">
-        <v>1300</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>670</v>
+        <v>34</v>
       </c>
       <c r="B7">
-        <v>430</v>
+        <v>22</v>
       </c>
       <c r="C7">
-        <v>890</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>510</v>
+        <v>26</v>
       </c>
       <c r="B8">
-        <v>1850</v>
+        <v>93</v>
       </c>
       <c r="C8">
-        <v>740</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>490</v>
+        <v>25</v>
       </c>
       <c r="B9">
-        <v>300</v>
+        <v>15</v>
       </c>
       <c r="C9">
-        <v>720</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>380</v>
+        <v>19</v>
       </c>
       <c r="B10">
-        <v>360</v>
+        <v>18</v>
       </c>
       <c r="C10">
-        <v>430</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>880</v>
+        <v>44</v>
       </c>
       <c r="B11">
-        <v>690</v>
+        <v>35</v>
       </c>
       <c r="C11">
-        <v>1050</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>